<commit_message>
Adjusted for New Level Requirements
</commit_message>
<xml_diff>
--- a/Cluster Settings/Misc/Level Information.xlsx
+++ b/Cluster Settings/Misc/Level Information.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaltP\Desktop\GitHub\ARK-Server\Cluster Settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaltP\Desktop\GitHub\ARK-Server\Cluster Settings\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="6">
   <si>
     <t>Level</t>
   </si>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q152"/>
+  <dimension ref="A1:Q262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="G152" sqref="G152"/>
+    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
+      <selection activeCell="H269" sqref="H269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6800,36 +6800,6 @@
         <f t="shared" si="14"/>
         <v>67280</v>
       </c>
-      <c r="I118">
-        <f t="shared" si="17"/>
-        <v>115</v>
-      </c>
-      <c r="J118">
-        <f t="shared" si="22"/>
-        <v>28185</v>
-      </c>
-      <c r="K118">
-        <f t="shared" si="18"/>
-        <v>886920</v>
-      </c>
-      <c r="M118">
-        <f t="shared" si="19"/>
-        <v>115</v>
-      </c>
-      <c r="N118" t="s">
-        <v>3</v>
-      </c>
-      <c r="O118">
-        <f t="shared" si="23"/>
-        <v>886920</v>
-      </c>
-      <c r="P118" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q118">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119">
@@ -6855,36 +6825,6 @@
         <f t="shared" si="14"/>
         <v>68445</v>
       </c>
-      <c r="I119">
-        <f t="shared" si="17"/>
-        <v>116</v>
-      </c>
-      <c r="J119">
-        <f t="shared" si="22"/>
-        <v>28865</v>
-      </c>
-      <c r="K119">
-        <f t="shared" si="18"/>
-        <v>915785</v>
-      </c>
-      <c r="M119">
-        <f t="shared" si="19"/>
-        <v>116</v>
-      </c>
-      <c r="N119" t="s">
-        <v>3</v>
-      </c>
-      <c r="O119">
-        <f t="shared" si="23"/>
-        <v>915785</v>
-      </c>
-      <c r="P119" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q119">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120">
@@ -6910,36 +6850,6 @@
         <f t="shared" si="14"/>
         <v>69620</v>
       </c>
-      <c r="I120">
-        <f t="shared" si="17"/>
-        <v>117</v>
-      </c>
-      <c r="J120">
-        <f t="shared" si="22"/>
-        <v>29545</v>
-      </c>
-      <c r="K120">
-        <f t="shared" si="18"/>
-        <v>945330</v>
-      </c>
-      <c r="M120">
-        <f t="shared" si="19"/>
-        <v>117</v>
-      </c>
-      <c r="N120" t="s">
-        <v>3</v>
-      </c>
-      <c r="O120">
-        <f t="shared" si="23"/>
-        <v>945330</v>
-      </c>
-      <c r="P120" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q120">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121">
@@ -6965,36 +6875,6 @@
         <f t="shared" si="14"/>
         <v>70805</v>
       </c>
-      <c r="I121">
-        <f t="shared" si="17"/>
-        <v>118</v>
-      </c>
-      <c r="J121">
-        <f t="shared" si="22"/>
-        <v>30225</v>
-      </c>
-      <c r="K121">
-        <f t="shared" si="18"/>
-        <v>975555</v>
-      </c>
-      <c r="M121">
-        <f t="shared" si="19"/>
-        <v>118</v>
-      </c>
-      <c r="N121" t="s">
-        <v>3</v>
-      </c>
-      <c r="O121">
-        <f t="shared" si="23"/>
-        <v>975555</v>
-      </c>
-      <c r="P121" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q121">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122">
@@ -7020,36 +6900,6 @@
         <f t="shared" si="14"/>
         <v>72000</v>
       </c>
-      <c r="I122">
-        <f t="shared" si="17"/>
-        <v>119</v>
-      </c>
-      <c r="J122">
-        <f t="shared" si="22"/>
-        <v>30905</v>
-      </c>
-      <c r="K122">
-        <f t="shared" si="18"/>
-        <v>1006460</v>
-      </c>
-      <c r="M122">
-        <f t="shared" si="19"/>
-        <v>119</v>
-      </c>
-      <c r="N122" t="s">
-        <v>3</v>
-      </c>
-      <c r="O122">
-        <f t="shared" si="23"/>
-        <v>1006460</v>
-      </c>
-      <c r="P122" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q122">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123">
@@ -7075,36 +6925,6 @@
         <f t="shared" si="14"/>
         <v>73205</v>
       </c>
-      <c r="I123">
-        <f t="shared" si="17"/>
-        <v>120</v>
-      </c>
-      <c r="J123">
-        <f>J122-J121+J122+120</f>
-        <v>31705</v>
-      </c>
-      <c r="K123">
-        <f t="shared" si="18"/>
-        <v>1038165</v>
-      </c>
-      <c r="M123">
-        <f t="shared" si="19"/>
-        <v>120</v>
-      </c>
-      <c r="N123" t="s">
-        <v>3</v>
-      </c>
-      <c r="O123">
-        <f t="shared" si="23"/>
-        <v>1038165</v>
-      </c>
-      <c r="P123" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q123">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124">
@@ -7130,36 +6950,6 @@
         <f t="shared" si="14"/>
         <v>74420</v>
       </c>
-      <c r="I124">
-        <f t="shared" si="17"/>
-        <v>121</v>
-      </c>
-      <c r="J124">
-        <f t="shared" si="22"/>
-        <v>32505</v>
-      </c>
-      <c r="K124">
-        <f t="shared" si="18"/>
-        <v>1070670</v>
-      </c>
-      <c r="M124">
-        <f t="shared" si="19"/>
-        <v>121</v>
-      </c>
-      <c r="N124" t="s">
-        <v>3</v>
-      </c>
-      <c r="O124">
-        <f t="shared" si="23"/>
-        <v>1070670</v>
-      </c>
-      <c r="P124" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q124">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125">
@@ -7185,36 +6975,6 @@
         <f t="shared" si="14"/>
         <v>75645</v>
       </c>
-      <c r="I125">
-        <f t="shared" si="17"/>
-        <v>122</v>
-      </c>
-      <c r="J125">
-        <f t="shared" si="22"/>
-        <v>33305</v>
-      </c>
-      <c r="K125">
-        <f t="shared" si="18"/>
-        <v>1103975</v>
-      </c>
-      <c r="M125">
-        <f t="shared" si="19"/>
-        <v>122</v>
-      </c>
-      <c r="N125" t="s">
-        <v>3</v>
-      </c>
-      <c r="O125">
-        <f t="shared" si="23"/>
-        <v>1103975</v>
-      </c>
-      <c r="P125" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q125">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126">
@@ -7240,36 +7000,6 @@
         <f t="shared" si="14"/>
         <v>76880</v>
       </c>
-      <c r="I126">
-        <f t="shared" si="17"/>
-        <v>123</v>
-      </c>
-      <c r="J126">
-        <f t="shared" si="22"/>
-        <v>34105</v>
-      </c>
-      <c r="K126">
-        <f t="shared" si="18"/>
-        <v>1138080</v>
-      </c>
-      <c r="M126">
-        <f t="shared" si="19"/>
-        <v>123</v>
-      </c>
-      <c r="N126" t="s">
-        <v>3</v>
-      </c>
-      <c r="O126">
-        <f t="shared" si="23"/>
-        <v>1138080</v>
-      </c>
-      <c r="P126" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q126">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127">
@@ -7295,36 +7025,6 @@
         <f t="shared" si="14"/>
         <v>78125</v>
       </c>
-      <c r="I127">
-        <f t="shared" si="17"/>
-        <v>124</v>
-      </c>
-      <c r="J127">
-        <f t="shared" si="22"/>
-        <v>34905</v>
-      </c>
-      <c r="K127">
-        <f t="shared" si="18"/>
-        <v>1172985</v>
-      </c>
-      <c r="M127">
-        <f t="shared" si="19"/>
-        <v>124</v>
-      </c>
-      <c r="N127" t="s">
-        <v>3</v>
-      </c>
-      <c r="O127">
-        <f t="shared" si="23"/>
-        <v>1172985</v>
-      </c>
-      <c r="P127" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q127">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128">
@@ -7350,38 +7050,8 @@
         <f t="shared" si="14"/>
         <v>79380</v>
       </c>
-      <c r="I128">
-        <f t="shared" si="17"/>
-        <v>125</v>
-      </c>
-      <c r="J128">
-        <f t="shared" si="22"/>
-        <v>35705</v>
-      </c>
-      <c r="K128">
-        <f t="shared" si="18"/>
-        <v>1208690</v>
-      </c>
-      <c r="M128">
-        <f t="shared" si="19"/>
-        <v>125</v>
-      </c>
-      <c r="N128" t="s">
-        <v>3</v>
-      </c>
-      <c r="O128">
-        <f t="shared" si="23"/>
-        <v>1208690</v>
-      </c>
-      <c r="P128" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q128">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
         <f t="shared" si="15"/>
         <v>126</v>
@@ -7405,38 +7075,8 @@
         <f t="shared" si="14"/>
         <v>80645</v>
       </c>
-      <c r="I129">
-        <f t="shared" si="17"/>
-        <v>126</v>
-      </c>
-      <c r="J129">
-        <f t="shared" si="22"/>
-        <v>36505</v>
-      </c>
-      <c r="K129">
-        <f t="shared" si="18"/>
-        <v>1245195</v>
-      </c>
-      <c r="M129">
-        <f t="shared" si="19"/>
-        <v>126</v>
-      </c>
-      <c r="N129" t="s">
-        <v>3</v>
-      </c>
-      <c r="O129">
-        <f t="shared" si="23"/>
-        <v>1245195</v>
-      </c>
-      <c r="P129" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q129">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
         <f t="shared" si="15"/>
         <v>127</v>
@@ -7460,38 +7100,8 @@
         <f t="shared" si="14"/>
         <v>81920</v>
       </c>
-      <c r="I130">
-        <f t="shared" si="17"/>
-        <v>127</v>
-      </c>
-      <c r="J130">
-        <f t="shared" si="22"/>
-        <v>37305</v>
-      </c>
-      <c r="K130">
-        <f t="shared" si="18"/>
-        <v>1282500</v>
-      </c>
-      <c r="M130">
-        <f t="shared" si="19"/>
-        <v>127</v>
-      </c>
-      <c r="N130" t="s">
-        <v>3</v>
-      </c>
-      <c r="O130">
-        <f t="shared" si="23"/>
-        <v>1282500</v>
-      </c>
-      <c r="P130" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q130">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
         <f t="shared" si="15"/>
         <v>128</v>
@@ -7515,38 +7125,8 @@
         <f t="shared" si="14"/>
         <v>83205</v>
       </c>
-      <c r="I131">
-        <f t="shared" si="17"/>
-        <v>128</v>
-      </c>
-      <c r="J131">
-        <f t="shared" si="22"/>
-        <v>38105</v>
-      </c>
-      <c r="K131">
-        <f t="shared" si="18"/>
-        <v>1320605</v>
-      </c>
-      <c r="M131">
-        <f t="shared" si="19"/>
-        <v>128</v>
-      </c>
-      <c r="N131" t="s">
-        <v>3</v>
-      </c>
-      <c r="O131">
-        <f t="shared" ref="O131:O151" si="24">K131</f>
-        <v>1320605</v>
-      </c>
-      <c r="P131" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q131">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" si="15"/>
         <v>129</v>
@@ -7560,50 +7140,20 @@
         <v>84500</v>
       </c>
       <c r="E132">
-        <f t="shared" ref="E132:E151" si="25">A132</f>
+        <f t="shared" ref="E132:E151" si="24">A132</f>
         <v>129</v>
       </c>
       <c r="F132" t="s">
         <v>3</v>
       </c>
       <c r="G132">
-        <f t="shared" ref="G132:G151" si="26">C132</f>
+        <f t="shared" ref="G132:G151" si="25">C132</f>
         <v>84500</v>
       </c>
-      <c r="I132">
-        <f t="shared" si="17"/>
-        <v>129</v>
-      </c>
-      <c r="J132">
-        <f t="shared" si="22"/>
-        <v>38905</v>
-      </c>
-      <c r="K132">
-        <f t="shared" si="18"/>
-        <v>1359510</v>
-      </c>
-      <c r="M132">
-        <f t="shared" si="19"/>
-        <v>129</v>
-      </c>
-      <c r="N132" t="s">
-        <v>3</v>
-      </c>
-      <c r="O132">
-        <f t="shared" si="24"/>
-        <v>1359510</v>
-      </c>
-      <c r="P132" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q132">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133">
-        <f t="shared" ref="A133:A152" si="27">A132+1</f>
+        <f t="shared" ref="A133:A196" si="26">A132+1</f>
         <v>130</v>
       </c>
       <c r="B133">
@@ -7611,1064 +7161,3244 @@
         <v>1305</v>
       </c>
       <c r="C133">
-        <f t="shared" ref="C133:C151" si="28">C132+B133</f>
+        <f t="shared" ref="C133:C151" si="27">C132+B133</f>
         <v>85805</v>
       </c>
       <c r="E133">
+        <f t="shared" si="24"/>
+        <v>130</v>
+      </c>
+      <c r="F133" t="s">
+        <v>3</v>
+      </c>
+      <c r="G133">
         <f t="shared" si="25"/>
-        <v>130</v>
-      </c>
-      <c r="F133" t="s">
-        <v>3</v>
-      </c>
-      <c r="G133">
+        <v>85805</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134">
         <f t="shared" si="26"/>
-        <v>85805</v>
-      </c>
-      <c r="I133">
-        <f t="shared" ref="I133:I151" si="29">I132+1</f>
-        <v>130</v>
-      </c>
-      <c r="J133">
-        <f>J132-J131+J132+130</f>
-        <v>39835</v>
-      </c>
-      <c r="K133">
-        <f t="shared" ref="K133:K151" si="30">K132+J133</f>
-        <v>1399345</v>
-      </c>
-      <c r="M133">
-        <f t="shared" ref="M133:M151" si="31">M132+1</f>
-        <v>130</v>
-      </c>
-      <c r="N133" t="s">
-        <v>3</v>
-      </c>
-      <c r="O133">
+        <v>131</v>
+      </c>
+      <c r="B134">
+        <f t="shared" ref="B134:B197" si="28">B133-B132+B133</f>
+        <v>1315</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="27"/>
+        <v>87120</v>
+      </c>
+      <c r="E134">
         <f t="shared" si="24"/>
-        <v>1399345</v>
-      </c>
-      <c r="P133" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q133">
-        <f t="shared" ref="Q133:Q151" si="32">Q132</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A134">
+        <v>131</v>
+      </c>
+      <c r="F134" t="s">
+        <v>3</v>
+      </c>
+      <c r="G134">
+        <f t="shared" si="25"/>
+        <v>87120</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <f t="shared" si="26"/>
+        <v>132</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="28"/>
+        <v>1325</v>
+      </c>
+      <c r="C135">
         <f t="shared" si="27"/>
-        <v>131</v>
-      </c>
-      <c r="B134">
-        <f t="shared" ref="B134:B152" si="33">B133-B132+B133</f>
-        <v>1315</v>
-      </c>
-      <c r="C134">
+        <v>88445</v>
+      </c>
+      <c r="E135">
+        <f t="shared" si="24"/>
+        <v>132</v>
+      </c>
+      <c r="F135" t="s">
+        <v>3</v>
+      </c>
+      <c r="G135">
+        <f t="shared" si="25"/>
+        <v>88445</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <f t="shared" si="26"/>
+        <v>133</v>
+      </c>
+      <c r="B136">
         <f t="shared" si="28"/>
-        <v>87120</v>
-      </c>
-      <c r="E134">
+        <v>1335</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="27"/>
+        <v>89780</v>
+      </c>
+      <c r="E136">
+        <f t="shared" si="24"/>
+        <v>133</v>
+      </c>
+      <c r="F136" t="s">
+        <v>3</v>
+      </c>
+      <c r="G136">
         <f t="shared" si="25"/>
-        <v>131</v>
-      </c>
-      <c r="F134" t="s">
-        <v>3</v>
-      </c>
-      <c r="G134">
+        <v>89780</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137">
         <f t="shared" si="26"/>
-        <v>87120</v>
-      </c>
-      <c r="I134">
-        <f t="shared" si="29"/>
-        <v>131</v>
-      </c>
-      <c r="J134">
-        <f t="shared" ref="J134:J151" si="34">J133-J132+J133</f>
-        <v>40765</v>
-      </c>
-      <c r="K134">
-        <f t="shared" si="30"/>
-        <v>1440110</v>
-      </c>
-      <c r="M134">
-        <f t="shared" si="31"/>
-        <v>131</v>
-      </c>
-      <c r="N134" t="s">
-        <v>3</v>
-      </c>
-      <c r="O134">
+        <v>134</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="28"/>
+        <v>1345</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="27"/>
+        <v>91125</v>
+      </c>
+      <c r="E137">
         <f t="shared" si="24"/>
-        <v>1440110</v>
-      </c>
-      <c r="P134" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q134">
+        <v>134</v>
+      </c>
+      <c r="F137" t="s">
+        <v>3</v>
+      </c>
+      <c r="G137">
+        <f t="shared" si="25"/>
+        <v>91125</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <f t="shared" si="26"/>
+        <v>135</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="28"/>
+        <v>1355</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="27"/>
+        <v>92480</v>
+      </c>
+      <c r="E138">
+        <f t="shared" si="24"/>
+        <v>135</v>
+      </c>
+      <c r="F138" t="s">
+        <v>3</v>
+      </c>
+      <c r="G138">
+        <f t="shared" si="25"/>
+        <v>92480</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <f t="shared" si="26"/>
+        <v>136</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="28"/>
+        <v>1365</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="27"/>
+        <v>93845</v>
+      </c>
+      <c r="E139">
+        <f t="shared" si="24"/>
+        <v>136</v>
+      </c>
+      <c r="F139" t="s">
+        <v>3</v>
+      </c>
+      <c r="G139">
+        <f t="shared" si="25"/>
+        <v>93845</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <f t="shared" si="26"/>
+        <v>137</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="28"/>
+        <v>1375</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="27"/>
+        <v>95220</v>
+      </c>
+      <c r="E140">
+        <f t="shared" si="24"/>
+        <v>137</v>
+      </c>
+      <c r="F140" t="s">
+        <v>3</v>
+      </c>
+      <c r="G140">
+        <f t="shared" si="25"/>
+        <v>95220</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <f t="shared" si="26"/>
+        <v>138</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="28"/>
+        <v>1385</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="27"/>
+        <v>96605</v>
+      </c>
+      <c r="E141">
+        <f t="shared" si="24"/>
+        <v>138</v>
+      </c>
+      <c r="F141" t="s">
+        <v>3</v>
+      </c>
+      <c r="G141">
+        <f t="shared" si="25"/>
+        <v>96605</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <f t="shared" si="26"/>
+        <v>139</v>
+      </c>
+      <c r="B142">
+        <f t="shared" si="28"/>
+        <v>1395</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="27"/>
+        <v>98000</v>
+      </c>
+      <c r="E142">
+        <f t="shared" si="24"/>
+        <v>139</v>
+      </c>
+      <c r="F142" t="s">
+        <v>3</v>
+      </c>
+      <c r="G142">
+        <f t="shared" si="25"/>
+        <v>98000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <f t="shared" si="26"/>
+        <v>140</v>
+      </c>
+      <c r="B143">
+        <f t="shared" si="28"/>
+        <v>1405</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="27"/>
+        <v>99405</v>
+      </c>
+      <c r="E143">
+        <f t="shared" si="24"/>
+        <v>140</v>
+      </c>
+      <c r="F143" t="s">
+        <v>3</v>
+      </c>
+      <c r="G143">
+        <f t="shared" si="25"/>
+        <v>99405</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <f t="shared" si="26"/>
+        <v>141</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="28"/>
+        <v>1415</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="27"/>
+        <v>100820</v>
+      </c>
+      <c r="E144">
+        <f t="shared" si="24"/>
+        <v>141</v>
+      </c>
+      <c r="F144" t="s">
+        <v>3</v>
+      </c>
+      <c r="G144">
+        <f t="shared" si="25"/>
+        <v>100820</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <f t="shared" si="26"/>
+        <v>142</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="28"/>
+        <v>1425</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="27"/>
+        <v>102245</v>
+      </c>
+      <c r="E145">
+        <f t="shared" si="24"/>
+        <v>142</v>
+      </c>
+      <c r="F145" t="s">
+        <v>3</v>
+      </c>
+      <c r="G145">
+        <f t="shared" si="25"/>
+        <v>102245</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <f t="shared" si="26"/>
+        <v>143</v>
+      </c>
+      <c r="B146">
+        <f t="shared" si="28"/>
+        <v>1435</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="27"/>
+        <v>103680</v>
+      </c>
+      <c r="E146">
+        <f t="shared" si="24"/>
+        <v>143</v>
+      </c>
+      <c r="F146" t="s">
+        <v>3</v>
+      </c>
+      <c r="G146">
+        <f t="shared" si="25"/>
+        <v>103680</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <f t="shared" si="26"/>
+        <v>144</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="28"/>
+        <v>1445</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="27"/>
+        <v>105125</v>
+      </c>
+      <c r="E147">
+        <f t="shared" si="24"/>
+        <v>144</v>
+      </c>
+      <c r="F147" t="s">
+        <v>3</v>
+      </c>
+      <c r="G147">
+        <f t="shared" si="25"/>
+        <v>105125</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <f t="shared" si="26"/>
+        <v>145</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="28"/>
+        <v>1455</v>
+      </c>
+      <c r="C148">
+        <f t="shared" si="27"/>
+        <v>106580</v>
+      </c>
+      <c r="E148">
+        <f t="shared" si="24"/>
+        <v>145</v>
+      </c>
+      <c r="F148" t="s">
+        <v>3</v>
+      </c>
+      <c r="G148">
+        <f t="shared" si="25"/>
+        <v>106580</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <f t="shared" si="26"/>
+        <v>146</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="28"/>
+        <v>1465</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="27"/>
+        <v>108045</v>
+      </c>
+      <c r="E149">
+        <f t="shared" si="24"/>
+        <v>146</v>
+      </c>
+      <c r="F149" t="s">
+        <v>3</v>
+      </c>
+      <c r="G149">
+        <f t="shared" si="25"/>
+        <v>108045</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <f t="shared" si="26"/>
+        <v>147</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="28"/>
+        <v>1475</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="27"/>
+        <v>109520</v>
+      </c>
+      <c r="E150">
+        <f t="shared" si="24"/>
+        <v>147</v>
+      </c>
+      <c r="F150" t="s">
+        <v>3</v>
+      </c>
+      <c r="G150">
+        <f t="shared" si="25"/>
+        <v>109520</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <f t="shared" si="26"/>
+        <v>148</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="28"/>
+        <v>1485</v>
+      </c>
+      <c r="C151">
+        <f t="shared" si="27"/>
+        <v>111005</v>
+      </c>
+      <c r="E151">
+        <f t="shared" si="24"/>
+        <v>148</v>
+      </c>
+      <c r="F151" t="s">
+        <v>3</v>
+      </c>
+      <c r="G151">
+        <f t="shared" si="25"/>
+        <v>111005</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <f t="shared" si="26"/>
+        <v>149</v>
+      </c>
+      <c r="B152">
+        <f t="shared" si="28"/>
+        <v>1495</v>
+      </c>
+      <c r="C152">
+        <f t="shared" ref="C152" si="29">C151+B152</f>
+        <v>112500</v>
+      </c>
+      <c r="E152">
+        <f t="shared" ref="E152" si="30">A152</f>
+        <v>149</v>
+      </c>
+      <c r="F152" t="s">
+        <v>3</v>
+      </c>
+      <c r="G152">
+        <f t="shared" ref="G152" si="31">C152</f>
+        <v>112500</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <f t="shared" si="26"/>
+        <v>150</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="28"/>
+        <v>1505</v>
+      </c>
+      <c r="C153">
+        <f t="shared" ref="C153:C216" si="32">C152+B153</f>
+        <v>114005</v>
+      </c>
+      <c r="E153">
+        <f t="shared" ref="E153:E216" si="33">A153</f>
+        <v>150</v>
+      </c>
+      <c r="F153" t="s">
+        <v>3</v>
+      </c>
+      <c r="G153">
+        <f t="shared" ref="G153:G216" si="34">C153</f>
+        <v>114005</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <f t="shared" si="26"/>
+        <v>151</v>
+      </c>
+      <c r="B154">
+        <f t="shared" si="28"/>
+        <v>1515</v>
+      </c>
+      <c r="C154">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A135">
-        <f t="shared" si="27"/>
-        <v>132</v>
-      </c>
-      <c r="B135">
+        <v>115520</v>
+      </c>
+      <c r="E154">
         <f t="shared" si="33"/>
-        <v>1325</v>
-      </c>
-      <c r="C135">
+        <v>151</v>
+      </c>
+      <c r="F154" t="s">
+        <v>3</v>
+      </c>
+      <c r="G154">
+        <f t="shared" si="34"/>
+        <v>115520</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <f t="shared" si="26"/>
+        <v>152</v>
+      </c>
+      <c r="B155">
         <f t="shared" si="28"/>
-        <v>88445</v>
-      </c>
-      <c r="E135">
-        <f t="shared" si="25"/>
-        <v>132</v>
-      </c>
-      <c r="F135" t="s">
-        <v>3</v>
-      </c>
-      <c r="G135">
+        <v>1525</v>
+      </c>
+      <c r="C155">
+        <f t="shared" si="32"/>
+        <v>117045</v>
+      </c>
+      <c r="E155">
+        <f t="shared" si="33"/>
+        <v>152</v>
+      </c>
+      <c r="F155" t="s">
+        <v>3</v>
+      </c>
+      <c r="G155">
+        <f t="shared" si="34"/>
+        <v>117045</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156">
         <f t="shared" si="26"/>
-        <v>88445</v>
-      </c>
-      <c r="I135">
-        <f t="shared" si="29"/>
-        <v>132</v>
-      </c>
-      <c r="J135">
+        <v>153</v>
+      </c>
+      <c r="B156">
+        <f t="shared" si="28"/>
+        <v>1535</v>
+      </c>
+      <c r="C156">
+        <f t="shared" si="32"/>
+        <v>118580</v>
+      </c>
+      <c r="E156">
+        <f t="shared" si="33"/>
+        <v>153</v>
+      </c>
+      <c r="F156" t="s">
+        <v>3</v>
+      </c>
+      <c r="G156">
         <f t="shared" si="34"/>
-        <v>41695</v>
-      </c>
-      <c r="K135">
-        <f t="shared" si="30"/>
-        <v>1481805</v>
-      </c>
-      <c r="M135">
-        <f t="shared" si="31"/>
-        <v>132</v>
-      </c>
-      <c r="N135" t="s">
-        <v>3</v>
-      </c>
-      <c r="O135">
-        <f t="shared" si="24"/>
-        <v>1481805</v>
-      </c>
-      <c r="P135" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q135">
+        <v>118580</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <f t="shared" si="26"/>
+        <v>154</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="28"/>
+        <v>1545</v>
+      </c>
+      <c r="C157">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A136">
-        <f t="shared" si="27"/>
-        <v>133</v>
-      </c>
-      <c r="B136">
+        <v>120125</v>
+      </c>
+      <c r="E157">
         <f t="shared" si="33"/>
-        <v>1335</v>
-      </c>
-      <c r="C136">
+        <v>154</v>
+      </c>
+      <c r="F157" t="s">
+        <v>3</v>
+      </c>
+      <c r="G157">
+        <f t="shared" si="34"/>
+        <v>120125</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <f t="shared" si="26"/>
+        <v>155</v>
+      </c>
+      <c r="B158">
         <f t="shared" si="28"/>
-        <v>89780</v>
-      </c>
-      <c r="E136">
-        <f t="shared" si="25"/>
-        <v>133</v>
-      </c>
-      <c r="F136" t="s">
-        <v>3</v>
-      </c>
-      <c r="G136">
+        <v>1555</v>
+      </c>
+      <c r="C158">
+        <f t="shared" si="32"/>
+        <v>121680</v>
+      </c>
+      <c r="E158">
+        <f t="shared" si="33"/>
+        <v>155</v>
+      </c>
+      <c r="F158" t="s">
+        <v>3</v>
+      </c>
+      <c r="G158">
+        <f t="shared" si="34"/>
+        <v>121680</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159">
         <f t="shared" si="26"/>
-        <v>89780</v>
-      </c>
-      <c r="I136">
-        <f t="shared" si="29"/>
-        <v>133</v>
-      </c>
-      <c r="J136">
+        <v>156</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="28"/>
+        <v>1565</v>
+      </c>
+      <c r="C159">
+        <f t="shared" si="32"/>
+        <v>123245</v>
+      </c>
+      <c r="E159">
+        <f t="shared" si="33"/>
+        <v>156</v>
+      </c>
+      <c r="F159" t="s">
+        <v>3</v>
+      </c>
+      <c r="G159">
         <f t="shared" si="34"/>
-        <v>42625</v>
-      </c>
-      <c r="K136">
-        <f t="shared" si="30"/>
-        <v>1524430</v>
-      </c>
-      <c r="M136">
-        <f t="shared" si="31"/>
-        <v>133</v>
-      </c>
-      <c r="N136" t="s">
-        <v>3</v>
-      </c>
-      <c r="O136">
-        <f t="shared" si="24"/>
-        <v>1524430</v>
-      </c>
-      <c r="P136" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q136">
+        <v>123245</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <f t="shared" si="26"/>
+        <v>157</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="28"/>
+        <v>1575</v>
+      </c>
+      <c r="C160">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A137">
-        <f t="shared" si="27"/>
-        <v>134</v>
-      </c>
-      <c r="B137">
+        <v>124820</v>
+      </c>
+      <c r="E160">
         <f t="shared" si="33"/>
-        <v>1345</v>
-      </c>
-      <c r="C137">
+        <v>157</v>
+      </c>
+      <c r="F160" t="s">
+        <v>3</v>
+      </c>
+      <c r="G160">
+        <f t="shared" si="34"/>
+        <v>124820</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <f t="shared" si="26"/>
+        <v>158</v>
+      </c>
+      <c r="B161">
         <f t="shared" si="28"/>
-        <v>91125</v>
-      </c>
-      <c r="E137">
-        <f t="shared" si="25"/>
-        <v>134</v>
-      </c>
-      <c r="F137" t="s">
-        <v>3</v>
-      </c>
-      <c r="G137">
+        <v>1585</v>
+      </c>
+      <c r="C161">
+        <f t="shared" si="32"/>
+        <v>126405</v>
+      </c>
+      <c r="E161">
+        <f t="shared" si="33"/>
+        <v>158</v>
+      </c>
+      <c r="F161" t="s">
+        <v>3</v>
+      </c>
+      <c r="G161">
+        <f t="shared" si="34"/>
+        <v>126405</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162">
         <f t="shared" si="26"/>
-        <v>91125</v>
-      </c>
-      <c r="I137">
-        <f t="shared" si="29"/>
-        <v>134</v>
-      </c>
-      <c r="J137">
+        <v>159</v>
+      </c>
+      <c r="B162">
+        <f t="shared" si="28"/>
+        <v>1595</v>
+      </c>
+      <c r="C162">
+        <f t="shared" si="32"/>
+        <v>128000</v>
+      </c>
+      <c r="E162">
+        <f t="shared" si="33"/>
+        <v>159</v>
+      </c>
+      <c r="F162" t="s">
+        <v>3</v>
+      </c>
+      <c r="G162">
         <f t="shared" si="34"/>
-        <v>43555</v>
-      </c>
-      <c r="K137">
-        <f t="shared" si="30"/>
-        <v>1567985</v>
-      </c>
-      <c r="M137">
-        <f t="shared" si="31"/>
-        <v>134</v>
-      </c>
-      <c r="N137" t="s">
-        <v>3</v>
-      </c>
-      <c r="O137">
-        <f t="shared" si="24"/>
-        <v>1567985</v>
-      </c>
-      <c r="P137" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q137">
+        <v>128000</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <f t="shared" si="26"/>
+        <v>160</v>
+      </c>
+      <c r="B163">
+        <f t="shared" si="28"/>
+        <v>1605</v>
+      </c>
+      <c r="C163">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A138">
-        <f t="shared" si="27"/>
-        <v>135</v>
-      </c>
-      <c r="B138">
+        <v>129605</v>
+      </c>
+      <c r="E163">
         <f t="shared" si="33"/>
-        <v>1355</v>
-      </c>
-      <c r="C138">
+        <v>160</v>
+      </c>
+      <c r="F163" t="s">
+        <v>3</v>
+      </c>
+      <c r="G163">
+        <f t="shared" si="34"/>
+        <v>129605</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <f t="shared" si="26"/>
+        <v>161</v>
+      </c>
+      <c r="B164">
         <f t="shared" si="28"/>
-        <v>92480</v>
-      </c>
-      <c r="E138">
-        <f t="shared" si="25"/>
-        <v>135</v>
-      </c>
-      <c r="F138" t="s">
-        <v>3</v>
-      </c>
-      <c r="G138">
+        <v>1615</v>
+      </c>
+      <c r="C164">
+        <f t="shared" si="32"/>
+        <v>131220</v>
+      </c>
+      <c r="E164">
+        <f t="shared" si="33"/>
+        <v>161</v>
+      </c>
+      <c r="F164" t="s">
+        <v>3</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="34"/>
+        <v>131220</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165">
         <f t="shared" si="26"/>
-        <v>92480</v>
-      </c>
-      <c r="I138">
-        <f t="shared" si="29"/>
-        <v>135</v>
-      </c>
-      <c r="J138">
+        <v>162</v>
+      </c>
+      <c r="B165">
+        <f t="shared" si="28"/>
+        <v>1625</v>
+      </c>
+      <c r="C165">
+        <f t="shared" si="32"/>
+        <v>132845</v>
+      </c>
+      <c r="E165">
+        <f t="shared" si="33"/>
+        <v>162</v>
+      </c>
+      <c r="F165" t="s">
+        <v>3</v>
+      </c>
+      <c r="G165">
         <f t="shared" si="34"/>
-        <v>44485</v>
-      </c>
-      <c r="K138">
-        <f t="shared" si="30"/>
-        <v>1612470</v>
-      </c>
-      <c r="M138">
-        <f t="shared" si="31"/>
-        <v>135</v>
-      </c>
-      <c r="N138" t="s">
-        <v>3</v>
-      </c>
-      <c r="O138">
-        <f t="shared" si="24"/>
-        <v>1612470</v>
-      </c>
-      <c r="P138" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q138">
+        <v>132845</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <f t="shared" si="26"/>
+        <v>163</v>
+      </c>
+      <c r="B166">
+        <f t="shared" si="28"/>
+        <v>1635</v>
+      </c>
+      <c r="C166">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A139">
-        <f t="shared" si="27"/>
-        <v>136</v>
-      </c>
-      <c r="B139">
+        <v>134480</v>
+      </c>
+      <c r="E166">
         <f t="shared" si="33"/>
-        <v>1365</v>
-      </c>
-      <c r="C139">
+        <v>163</v>
+      </c>
+      <c r="F166" t="s">
+        <v>3</v>
+      </c>
+      <c r="G166">
+        <f t="shared" si="34"/>
+        <v>134480</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <f t="shared" si="26"/>
+        <v>164</v>
+      </c>
+      <c r="B167">
         <f t="shared" si="28"/>
-        <v>93845</v>
-      </c>
-      <c r="E139">
-        <f t="shared" si="25"/>
-        <v>136</v>
-      </c>
-      <c r="F139" t="s">
-        <v>3</v>
-      </c>
-      <c r="G139">
+        <v>1645</v>
+      </c>
+      <c r="C167">
+        <f t="shared" si="32"/>
+        <v>136125</v>
+      </c>
+      <c r="E167">
+        <f t="shared" si="33"/>
+        <v>164</v>
+      </c>
+      <c r="F167" t="s">
+        <v>3</v>
+      </c>
+      <c r="G167">
+        <f t="shared" si="34"/>
+        <v>136125</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168">
         <f t="shared" si="26"/>
-        <v>93845</v>
-      </c>
-      <c r="I139">
-        <f t="shared" si="29"/>
-        <v>136</v>
-      </c>
-      <c r="J139">
+        <v>165</v>
+      </c>
+      <c r="B168">
+        <f t="shared" si="28"/>
+        <v>1655</v>
+      </c>
+      <c r="C168">
+        <f t="shared" si="32"/>
+        <v>137780</v>
+      </c>
+      <c r="E168">
+        <f t="shared" si="33"/>
+        <v>165</v>
+      </c>
+      <c r="F168" t="s">
+        <v>3</v>
+      </c>
+      <c r="G168">
         <f t="shared" si="34"/>
-        <v>45415</v>
-      </c>
-      <c r="K139">
-        <f t="shared" si="30"/>
-        <v>1657885</v>
-      </c>
-      <c r="M139">
-        <f t="shared" si="31"/>
-        <v>136</v>
-      </c>
-      <c r="N139" t="s">
-        <v>3</v>
-      </c>
-      <c r="O139">
-        <f t="shared" si="24"/>
-        <v>1657885</v>
-      </c>
-      <c r="P139" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q139">
+        <v>137780</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <f t="shared" si="26"/>
+        <v>166</v>
+      </c>
+      <c r="B169">
+        <f t="shared" si="28"/>
+        <v>1665</v>
+      </c>
+      <c r="C169">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A140">
-        <f t="shared" si="27"/>
-        <v>137</v>
-      </c>
-      <c r="B140">
+        <v>139445</v>
+      </c>
+      <c r="E169">
         <f t="shared" si="33"/>
-        <v>1375</v>
-      </c>
-      <c r="C140">
+        <v>166</v>
+      </c>
+      <c r="F169" t="s">
+        <v>3</v>
+      </c>
+      <c r="G169">
+        <f t="shared" si="34"/>
+        <v>139445</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <f t="shared" si="26"/>
+        <v>167</v>
+      </c>
+      <c r="B170">
         <f t="shared" si="28"/>
-        <v>95220</v>
-      </c>
-      <c r="E140">
-        <f t="shared" si="25"/>
-        <v>137</v>
-      </c>
-      <c r="F140" t="s">
-        <v>3</v>
-      </c>
-      <c r="G140">
+        <v>1675</v>
+      </c>
+      <c r="C170">
+        <f t="shared" si="32"/>
+        <v>141120</v>
+      </c>
+      <c r="E170">
+        <f t="shared" si="33"/>
+        <v>167</v>
+      </c>
+      <c r="F170" t="s">
+        <v>3</v>
+      </c>
+      <c r="G170">
+        <f t="shared" si="34"/>
+        <v>141120</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171">
         <f t="shared" si="26"/>
-        <v>95220</v>
-      </c>
-      <c r="I140">
-        <f t="shared" si="29"/>
-        <v>137</v>
-      </c>
-      <c r="J140">
+        <v>168</v>
+      </c>
+      <c r="B171">
+        <f t="shared" si="28"/>
+        <v>1685</v>
+      </c>
+      <c r="C171">
+        <f t="shared" si="32"/>
+        <v>142805</v>
+      </c>
+      <c r="E171">
+        <f t="shared" si="33"/>
+        <v>168</v>
+      </c>
+      <c r="F171" t="s">
+        <v>3</v>
+      </c>
+      <c r="G171">
         <f t="shared" si="34"/>
-        <v>46345</v>
-      </c>
-      <c r="K140">
-        <f t="shared" si="30"/>
-        <v>1704230</v>
-      </c>
-      <c r="M140">
-        <f t="shared" si="31"/>
-        <v>137</v>
-      </c>
-      <c r="N140" t="s">
-        <v>3</v>
-      </c>
-      <c r="O140">
-        <f t="shared" si="24"/>
-        <v>1704230</v>
-      </c>
-      <c r="P140" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q140">
+        <v>142805</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <f t="shared" si="26"/>
+        <v>169</v>
+      </c>
+      <c r="B172">
+        <f t="shared" si="28"/>
+        <v>1695</v>
+      </c>
+      <c r="C172">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A141">
-        <f t="shared" si="27"/>
-        <v>138</v>
-      </c>
-      <c r="B141">
+        <v>144500</v>
+      </c>
+      <c r="E172">
         <f t="shared" si="33"/>
-        <v>1385</v>
-      </c>
-      <c r="C141">
+        <v>169</v>
+      </c>
+      <c r="F172" t="s">
+        <v>3</v>
+      </c>
+      <c r="G172">
+        <f t="shared" si="34"/>
+        <v>144500</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <f t="shared" si="26"/>
+        <v>170</v>
+      </c>
+      <c r="B173">
         <f t="shared" si="28"/>
-        <v>96605</v>
-      </c>
-      <c r="E141">
-        <f t="shared" si="25"/>
-        <v>138</v>
-      </c>
-      <c r="F141" t="s">
-        <v>3</v>
-      </c>
-      <c r="G141">
+        <v>1705</v>
+      </c>
+      <c r="C173">
+        <f t="shared" si="32"/>
+        <v>146205</v>
+      </c>
+      <c r="E173">
+        <f t="shared" si="33"/>
+        <v>170</v>
+      </c>
+      <c r="F173" t="s">
+        <v>3</v>
+      </c>
+      <c r="G173">
+        <f t="shared" si="34"/>
+        <v>146205</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174">
         <f t="shared" si="26"/>
-        <v>96605</v>
-      </c>
-      <c r="I141">
-        <f t="shared" si="29"/>
-        <v>138</v>
-      </c>
-      <c r="J141">
+        <v>171</v>
+      </c>
+      <c r="B174">
+        <f t="shared" si="28"/>
+        <v>1715</v>
+      </c>
+      <c r="C174">
+        <f t="shared" si="32"/>
+        <v>147920</v>
+      </c>
+      <c r="E174">
+        <f t="shared" si="33"/>
+        <v>171</v>
+      </c>
+      <c r="F174" t="s">
+        <v>3</v>
+      </c>
+      <c r="G174">
         <f t="shared" si="34"/>
-        <v>47275</v>
-      </c>
-      <c r="K141">
-        <f t="shared" si="30"/>
-        <v>1751505</v>
-      </c>
-      <c r="M141">
-        <f t="shared" si="31"/>
-        <v>138</v>
-      </c>
-      <c r="N141" t="s">
-        <v>3</v>
-      </c>
-      <c r="O141">
-        <f t="shared" si="24"/>
-        <v>1751505</v>
-      </c>
-      <c r="P141" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q141">
+        <v>147920</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <f t="shared" si="26"/>
+        <v>172</v>
+      </c>
+      <c r="B175">
+        <f t="shared" si="28"/>
+        <v>1725</v>
+      </c>
+      <c r="C175">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A142">
-        <f t="shared" si="27"/>
-        <v>139</v>
-      </c>
-      <c r="B142">
+        <v>149645</v>
+      </c>
+      <c r="E175">
         <f t="shared" si="33"/>
-        <v>1395</v>
-      </c>
-      <c r="C142">
+        <v>172</v>
+      </c>
+      <c r="F175" t="s">
+        <v>3</v>
+      </c>
+      <c r="G175">
+        <f t="shared" si="34"/>
+        <v>149645</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <f t="shared" si="26"/>
+        <v>173</v>
+      </c>
+      <c r="B176">
         <f t="shared" si="28"/>
-        <v>98000</v>
-      </c>
-      <c r="E142">
-        <f t="shared" si="25"/>
-        <v>139</v>
-      </c>
-      <c r="F142" t="s">
-        <v>3</v>
-      </c>
-      <c r="G142">
+        <v>1735</v>
+      </c>
+      <c r="C176">
+        <f t="shared" si="32"/>
+        <v>151380</v>
+      </c>
+      <c r="E176">
+        <f t="shared" si="33"/>
+        <v>173</v>
+      </c>
+      <c r="F176" t="s">
+        <v>3</v>
+      </c>
+      <c r="G176">
+        <f t="shared" si="34"/>
+        <v>151380</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177">
         <f t="shared" si="26"/>
-        <v>98000</v>
-      </c>
-      <c r="I142">
-        <f t="shared" si="29"/>
-        <v>139</v>
-      </c>
-      <c r="J142">
+        <v>174</v>
+      </c>
+      <c r="B177">
+        <f t="shared" si="28"/>
+        <v>1745</v>
+      </c>
+      <c r="C177">
+        <f t="shared" si="32"/>
+        <v>153125</v>
+      </c>
+      <c r="E177">
+        <f t="shared" si="33"/>
+        <v>174</v>
+      </c>
+      <c r="F177" t="s">
+        <v>3</v>
+      </c>
+      <c r="G177">
         <f t="shared" si="34"/>
-        <v>48205</v>
-      </c>
-      <c r="K142">
-        <f t="shared" si="30"/>
-        <v>1799710</v>
-      </c>
-      <c r="M142">
-        <f t="shared" si="31"/>
-        <v>139</v>
-      </c>
-      <c r="N142" t="s">
-        <v>3</v>
-      </c>
-      <c r="O142">
-        <f t="shared" si="24"/>
-        <v>1799710</v>
-      </c>
-      <c r="P142" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q142">
+        <v>153125</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <f t="shared" si="26"/>
+        <v>175</v>
+      </c>
+      <c r="B178">
+        <f t="shared" si="28"/>
+        <v>1755</v>
+      </c>
+      <c r="C178">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A143">
-        <f t="shared" si="27"/>
-        <v>140</v>
-      </c>
-      <c r="B143">
+        <v>154880</v>
+      </c>
+      <c r="E178">
         <f t="shared" si="33"/>
-        <v>1405</v>
-      </c>
-      <c r="C143">
+        <v>175</v>
+      </c>
+      <c r="F178" t="s">
+        <v>3</v>
+      </c>
+      <c r="G178">
+        <f t="shared" si="34"/>
+        <v>154880</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <f t="shared" si="26"/>
+        <v>176</v>
+      </c>
+      <c r="B179">
         <f t="shared" si="28"/>
-        <v>99405</v>
-      </c>
-      <c r="E143">
-        <f t="shared" si="25"/>
-        <v>140</v>
-      </c>
-      <c r="F143" t="s">
-        <v>3</v>
-      </c>
-      <c r="G143">
+        <v>1765</v>
+      </c>
+      <c r="C179">
+        <f t="shared" si="32"/>
+        <v>156645</v>
+      </c>
+      <c r="E179">
+        <f t="shared" si="33"/>
+        <v>176</v>
+      </c>
+      <c r="F179" t="s">
+        <v>3</v>
+      </c>
+      <c r="G179">
+        <f t="shared" si="34"/>
+        <v>156645</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180">
         <f t="shared" si="26"/>
-        <v>99405</v>
-      </c>
-      <c r="I143">
-        <f t="shared" si="29"/>
-        <v>140</v>
-      </c>
-      <c r="J143">
-        <f>J142-J141+J142+140</f>
-        <v>49275</v>
-      </c>
-      <c r="K143">
-        <f t="shared" si="30"/>
-        <v>1848985</v>
-      </c>
-      <c r="M143">
-        <f t="shared" si="31"/>
-        <v>140</v>
-      </c>
-      <c r="N143" t="s">
-        <v>3</v>
-      </c>
-      <c r="O143">
-        <f t="shared" si="24"/>
-        <v>1848985</v>
-      </c>
-      <c r="P143" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q143">
+        <v>177</v>
+      </c>
+      <c r="B180">
+        <f t="shared" si="28"/>
+        <v>1775</v>
+      </c>
+      <c r="C180">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <f t="shared" si="27"/>
-        <v>141</v>
-      </c>
-      <c r="B144">
+        <v>158420</v>
+      </c>
+      <c r="E180">
         <f t="shared" si="33"/>
-        <v>1415</v>
-      </c>
-      <c r="C144">
+        <v>177</v>
+      </c>
+      <c r="F180" t="s">
+        <v>3</v>
+      </c>
+      <c r="G180">
+        <f t="shared" si="34"/>
+        <v>158420</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <f t="shared" si="26"/>
+        <v>178</v>
+      </c>
+      <c r="B181">
         <f t="shared" si="28"/>
-        <v>100820</v>
-      </c>
-      <c r="E144">
-        <f t="shared" si="25"/>
-        <v>141</v>
-      </c>
-      <c r="F144" t="s">
-        <v>3</v>
-      </c>
-      <c r="G144">
+        <v>1785</v>
+      </c>
+      <c r="C181">
+        <f t="shared" si="32"/>
+        <v>160205</v>
+      </c>
+      <c r="E181">
+        <f t="shared" si="33"/>
+        <v>178</v>
+      </c>
+      <c r="F181" t="s">
+        <v>3</v>
+      </c>
+      <c r="G181">
+        <f t="shared" si="34"/>
+        <v>160205</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182">
         <f t="shared" si="26"/>
-        <v>100820</v>
-      </c>
-      <c r="I144">
-        <f t="shared" si="29"/>
-        <v>141</v>
-      </c>
-      <c r="J144">
+        <v>179</v>
+      </c>
+      <c r="B182">
+        <f t="shared" si="28"/>
+        <v>1795</v>
+      </c>
+      <c r="C182">
+        <f t="shared" si="32"/>
+        <v>162000</v>
+      </c>
+      <c r="E182">
+        <f t="shared" si="33"/>
+        <v>179</v>
+      </c>
+      <c r="F182" t="s">
+        <v>3</v>
+      </c>
+      <c r="G182">
         <f t="shared" si="34"/>
-        <v>50345</v>
-      </c>
-      <c r="K144">
-        <f t="shared" si="30"/>
-        <v>1899330</v>
-      </c>
-      <c r="M144">
-        <f t="shared" si="31"/>
-        <v>141</v>
-      </c>
-      <c r="N144" t="s">
-        <v>3</v>
-      </c>
-      <c r="O144">
-        <f t="shared" si="24"/>
-        <v>1899330</v>
-      </c>
-      <c r="P144" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q144">
+        <v>162000</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <f t="shared" si="26"/>
+        <v>180</v>
+      </c>
+      <c r="B183">
+        <f t="shared" si="28"/>
+        <v>1805</v>
+      </c>
+      <c r="C183">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <f t="shared" si="27"/>
-        <v>142</v>
-      </c>
-      <c r="B145">
+        <v>163805</v>
+      </c>
+      <c r="E183">
         <f t="shared" si="33"/>
-        <v>1425</v>
-      </c>
-      <c r="C145">
+        <v>180</v>
+      </c>
+      <c r="F183" t="s">
+        <v>3</v>
+      </c>
+      <c r="G183">
+        <f t="shared" si="34"/>
+        <v>163805</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <f t="shared" si="26"/>
+        <v>181</v>
+      </c>
+      <c r="B184">
         <f t="shared" si="28"/>
-        <v>102245</v>
-      </c>
-      <c r="E145">
-        <f t="shared" si="25"/>
-        <v>142</v>
-      </c>
-      <c r="F145" t="s">
-        <v>3</v>
-      </c>
-      <c r="G145">
+        <v>1815</v>
+      </c>
+      <c r="C184">
+        <f t="shared" si="32"/>
+        <v>165620</v>
+      </c>
+      <c r="E184">
+        <f t="shared" si="33"/>
+        <v>181</v>
+      </c>
+      <c r="F184" t="s">
+        <v>3</v>
+      </c>
+      <c r="G184">
+        <f t="shared" si="34"/>
+        <v>165620</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185">
         <f t="shared" si="26"/>
-        <v>102245</v>
-      </c>
-      <c r="I145">
-        <f t="shared" si="29"/>
-        <v>142</v>
-      </c>
-      <c r="J145">
+        <v>182</v>
+      </c>
+      <c r="B185">
+        <f t="shared" si="28"/>
+        <v>1825</v>
+      </c>
+      <c r="C185">
+        <f t="shared" si="32"/>
+        <v>167445</v>
+      </c>
+      <c r="E185">
+        <f t="shared" si="33"/>
+        <v>182</v>
+      </c>
+      <c r="F185" t="s">
+        <v>3</v>
+      </c>
+      <c r="G185">
         <f t="shared" si="34"/>
-        <v>51415</v>
-      </c>
-      <c r="K145">
-        <f t="shared" si="30"/>
-        <v>1950745</v>
-      </c>
-      <c r="M145">
-        <f t="shared" si="31"/>
-        <v>142</v>
-      </c>
-      <c r="N145" t="s">
-        <v>3</v>
-      </c>
-      <c r="O145">
-        <f t="shared" si="24"/>
-        <v>1950745</v>
-      </c>
-      <c r="P145" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q145">
+        <v>167445</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <f t="shared" si="26"/>
+        <v>183</v>
+      </c>
+      <c r="B186">
+        <f t="shared" si="28"/>
+        <v>1835</v>
+      </c>
+      <c r="C186">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <f t="shared" si="27"/>
-        <v>143</v>
-      </c>
-      <c r="B146">
+        <v>169280</v>
+      </c>
+      <c r="E186">
         <f t="shared" si="33"/>
-        <v>1435</v>
-      </c>
-      <c r="C146">
+        <v>183</v>
+      </c>
+      <c r="F186" t="s">
+        <v>3</v>
+      </c>
+      <c r="G186">
+        <f t="shared" si="34"/>
+        <v>169280</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <f t="shared" si="26"/>
+        <v>184</v>
+      </c>
+      <c r="B187">
         <f t="shared" si="28"/>
-        <v>103680</v>
-      </c>
-      <c r="E146">
-        <f t="shared" si="25"/>
-        <v>143</v>
-      </c>
-      <c r="F146" t="s">
-        <v>3</v>
-      </c>
-      <c r="G146">
+        <v>1845</v>
+      </c>
+      <c r="C187">
+        <f t="shared" si="32"/>
+        <v>171125</v>
+      </c>
+      <c r="E187">
+        <f t="shared" si="33"/>
+        <v>184</v>
+      </c>
+      <c r="F187" t="s">
+        <v>3</v>
+      </c>
+      <c r="G187">
+        <f t="shared" si="34"/>
+        <v>171125</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188">
         <f t="shared" si="26"/>
-        <v>103680</v>
-      </c>
-      <c r="I146">
-        <f t="shared" si="29"/>
-        <v>143</v>
-      </c>
-      <c r="J146">
+        <v>185</v>
+      </c>
+      <c r="B188">
+        <f t="shared" si="28"/>
+        <v>1855</v>
+      </c>
+      <c r="C188">
+        <f t="shared" si="32"/>
+        <v>172980</v>
+      </c>
+      <c r="E188">
+        <f t="shared" si="33"/>
+        <v>185</v>
+      </c>
+      <c r="F188" t="s">
+        <v>3</v>
+      </c>
+      <c r="G188">
         <f t="shared" si="34"/>
-        <v>52485</v>
-      </c>
-      <c r="K146">
-        <f t="shared" si="30"/>
-        <v>2003230</v>
-      </c>
-      <c r="M146">
-        <f t="shared" si="31"/>
-        <v>143</v>
-      </c>
-      <c r="N146" t="s">
-        <v>3</v>
-      </c>
-      <c r="O146">
-        <f t="shared" si="24"/>
-        <v>2003230</v>
-      </c>
-      <c r="P146" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q146">
+        <v>172980</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <f t="shared" si="26"/>
+        <v>186</v>
+      </c>
+      <c r="B189">
+        <f t="shared" si="28"/>
+        <v>1865</v>
+      </c>
+      <c r="C189">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <f t="shared" si="27"/>
-        <v>144</v>
-      </c>
-      <c r="B147">
+        <v>174845</v>
+      </c>
+      <c r="E189">
         <f t="shared" si="33"/>
-        <v>1445</v>
-      </c>
-      <c r="C147">
+        <v>186</v>
+      </c>
+      <c r="F189" t="s">
+        <v>3</v>
+      </c>
+      <c r="G189">
+        <f t="shared" si="34"/>
+        <v>174845</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <f t="shared" si="26"/>
+        <v>187</v>
+      </c>
+      <c r="B190">
         <f t="shared" si="28"/>
-        <v>105125</v>
-      </c>
-      <c r="E147">
-        <f t="shared" si="25"/>
-        <v>144</v>
-      </c>
-      <c r="F147" t="s">
-        <v>3</v>
-      </c>
-      <c r="G147">
+        <v>1875</v>
+      </c>
+      <c r="C190">
+        <f t="shared" si="32"/>
+        <v>176720</v>
+      </c>
+      <c r="E190">
+        <f t="shared" si="33"/>
+        <v>187</v>
+      </c>
+      <c r="F190" t="s">
+        <v>3</v>
+      </c>
+      <c r="G190">
+        <f t="shared" si="34"/>
+        <v>176720</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191">
         <f t="shared" si="26"/>
-        <v>105125</v>
-      </c>
-      <c r="I147">
-        <f t="shared" si="29"/>
-        <v>144</v>
-      </c>
-      <c r="J147">
+        <v>188</v>
+      </c>
+      <c r="B191">
+        <f t="shared" si="28"/>
+        <v>1885</v>
+      </c>
+      <c r="C191">
+        <f t="shared" si="32"/>
+        <v>178605</v>
+      </c>
+      <c r="E191">
+        <f t="shared" si="33"/>
+        <v>188</v>
+      </c>
+      <c r="F191" t="s">
+        <v>3</v>
+      </c>
+      <c r="G191">
         <f t="shared" si="34"/>
-        <v>53555</v>
-      </c>
-      <c r="K147">
-        <f t="shared" si="30"/>
-        <v>2056785</v>
-      </c>
-      <c r="M147">
-        <f t="shared" si="31"/>
-        <v>144</v>
-      </c>
-      <c r="N147" t="s">
-        <v>3</v>
-      </c>
-      <c r="O147">
-        <f t="shared" si="24"/>
-        <v>2056785</v>
-      </c>
-      <c r="P147" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q147">
+        <v>178605</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <f t="shared" si="26"/>
+        <v>189</v>
+      </c>
+      <c r="B192">
+        <f t="shared" si="28"/>
+        <v>1895</v>
+      </c>
+      <c r="C192">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A148">
-        <f t="shared" si="27"/>
-        <v>145</v>
-      </c>
-      <c r="B148">
+        <v>180500</v>
+      </c>
+      <c r="E192">
         <f t="shared" si="33"/>
-        <v>1455</v>
-      </c>
-      <c r="C148">
+        <v>189</v>
+      </c>
+      <c r="F192" t="s">
+        <v>3</v>
+      </c>
+      <c r="G192">
+        <f t="shared" si="34"/>
+        <v>180500</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <f t="shared" si="26"/>
+        <v>190</v>
+      </c>
+      <c r="B193">
         <f t="shared" si="28"/>
-        <v>106580</v>
-      </c>
-      <c r="E148">
-        <f t="shared" si="25"/>
-        <v>145</v>
-      </c>
-      <c r="F148" t="s">
-        <v>3</v>
-      </c>
-      <c r="G148">
+        <v>1905</v>
+      </c>
+      <c r="C193">
+        <f t="shared" si="32"/>
+        <v>182405</v>
+      </c>
+      <c r="E193">
+        <f t="shared" si="33"/>
+        <v>190</v>
+      </c>
+      <c r="F193" t="s">
+        <v>3</v>
+      </c>
+      <c r="G193">
+        <f t="shared" si="34"/>
+        <v>182405</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194">
         <f t="shared" si="26"/>
-        <v>106580</v>
-      </c>
-      <c r="I148">
-        <f t="shared" si="29"/>
-        <v>145</v>
-      </c>
-      <c r="J148">
+        <v>191</v>
+      </c>
+      <c r="B194">
+        <f t="shared" si="28"/>
+        <v>1915</v>
+      </c>
+      <c r="C194">
+        <f t="shared" si="32"/>
+        <v>184320</v>
+      </c>
+      <c r="E194">
+        <f t="shared" si="33"/>
+        <v>191</v>
+      </c>
+      <c r="F194" t="s">
+        <v>3</v>
+      </c>
+      <c r="G194">
         <f t="shared" si="34"/>
-        <v>54625</v>
-      </c>
-      <c r="K148">
-        <f t="shared" si="30"/>
-        <v>2111410</v>
-      </c>
-      <c r="M148">
-        <f t="shared" si="31"/>
-        <v>145</v>
-      </c>
-      <c r="N148" t="s">
-        <v>3</v>
-      </c>
-      <c r="O148">
-        <f t="shared" si="24"/>
-        <v>2111410</v>
-      </c>
-      <c r="P148" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q148">
+        <v>184320</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <f t="shared" si="26"/>
+        <v>192</v>
+      </c>
+      <c r="B195">
+        <f t="shared" si="28"/>
+        <v>1925</v>
+      </c>
+      <c r="C195">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A149">
-        <f t="shared" si="27"/>
-        <v>146</v>
-      </c>
-      <c r="B149">
+        <v>186245</v>
+      </c>
+      <c r="E195">
         <f t="shared" si="33"/>
-        <v>1465</v>
-      </c>
-      <c r="C149">
+        <v>192</v>
+      </c>
+      <c r="F195" t="s">
+        <v>3</v>
+      </c>
+      <c r="G195">
+        <f t="shared" si="34"/>
+        <v>186245</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <f t="shared" si="26"/>
+        <v>193</v>
+      </c>
+      <c r="B196">
         <f t="shared" si="28"/>
-        <v>108045</v>
-      </c>
-      <c r="E149">
-        <f t="shared" si="25"/>
-        <v>146</v>
-      </c>
-      <c r="F149" t="s">
-        <v>3</v>
-      </c>
-      <c r="G149">
-        <f t="shared" si="26"/>
-        <v>108045</v>
-      </c>
-      <c r="I149">
-        <f t="shared" si="29"/>
-        <v>146</v>
-      </c>
-      <c r="J149">
+        <v>1935</v>
+      </c>
+      <c r="C196">
+        <f t="shared" si="32"/>
+        <v>188180</v>
+      </c>
+      <c r="E196">
+        <f t="shared" si="33"/>
+        <v>193</v>
+      </c>
+      <c r="F196" t="s">
+        <v>3</v>
+      </c>
+      <c r="G196">
         <f t="shared" si="34"/>
-        <v>55695</v>
-      </c>
-      <c r="K149">
-        <f t="shared" si="30"/>
-        <v>2167105</v>
-      </c>
-      <c r="M149">
-        <f t="shared" si="31"/>
-        <v>146</v>
-      </c>
-      <c r="N149" t="s">
-        <v>3</v>
-      </c>
-      <c r="O149">
-        <f t="shared" si="24"/>
-        <v>2167105</v>
-      </c>
-      <c r="P149" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q149">
+        <v>188180</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <f t="shared" ref="A197:A260" si="35">A196+1</f>
+        <v>194</v>
+      </c>
+      <c r="B197">
+        <f t="shared" si="28"/>
+        <v>1945</v>
+      </c>
+      <c r="C197">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A150">
-        <f t="shared" si="27"/>
-        <v>147</v>
-      </c>
-      <c r="B150">
+        <v>190125</v>
+      </c>
+      <c r="E197">
         <f t="shared" si="33"/>
-        <v>1475</v>
-      </c>
-      <c r="C150">
-        <f t="shared" si="28"/>
-        <v>109520</v>
-      </c>
-      <c r="E150">
-        <f t="shared" si="25"/>
-        <v>147</v>
-      </c>
-      <c r="F150" t="s">
-        <v>3</v>
-      </c>
-      <c r="G150">
-        <f t="shared" si="26"/>
-        <v>109520</v>
-      </c>
-      <c r="I150">
-        <f t="shared" si="29"/>
-        <v>147</v>
-      </c>
-      <c r="J150">
+        <v>194</v>
+      </c>
+      <c r="F197" t="s">
+        <v>3</v>
+      </c>
+      <c r="G197">
         <f t="shared" si="34"/>
-        <v>56765</v>
-      </c>
-      <c r="K150">
-        <f t="shared" si="30"/>
-        <v>2223870</v>
-      </c>
-      <c r="M150">
-        <f t="shared" si="31"/>
-        <v>147</v>
-      </c>
-      <c r="N150" t="s">
-        <v>3</v>
-      </c>
-      <c r="O150">
-        <f t="shared" si="24"/>
-        <v>2223870</v>
-      </c>
-      <c r="P150" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q150">
+        <v>190125</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <f t="shared" si="35"/>
+        <v>195</v>
+      </c>
+      <c r="B198">
+        <f t="shared" ref="B198:B261" si="36">B197-B196+B197</f>
+        <v>1955</v>
+      </c>
+      <c r="C198">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A151">
-        <f t="shared" si="27"/>
-        <v>148</v>
-      </c>
-      <c r="B151">
+        <v>192080</v>
+      </c>
+      <c r="E198">
         <f t="shared" si="33"/>
-        <v>1485</v>
-      </c>
-      <c r="C151">
-        <f t="shared" si="28"/>
-        <v>111005</v>
-      </c>
-      <c r="E151">
-        <f t="shared" si="25"/>
-        <v>148</v>
-      </c>
-      <c r="F151" t="s">
-        <v>3</v>
-      </c>
-      <c r="G151">
-        <f t="shared" si="26"/>
-        <v>111005</v>
-      </c>
-      <c r="I151">
-        <f t="shared" si="29"/>
-        <v>148</v>
-      </c>
-      <c r="J151">
+        <v>195</v>
+      </c>
+      <c r="F198" t="s">
+        <v>3</v>
+      </c>
+      <c r="G198">
         <f t="shared" si="34"/>
-        <v>57835</v>
-      </c>
-      <c r="K151">
-        <f t="shared" si="30"/>
-        <v>2281705</v>
-      </c>
-      <c r="M151">
-        <f t="shared" si="31"/>
-        <v>148</v>
-      </c>
-      <c r="N151" t="s">
-        <v>3</v>
-      </c>
-      <c r="O151">
-        <f t="shared" si="24"/>
-        <v>2281705</v>
-      </c>
-      <c r="P151" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q151">
+        <v>192080</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <f t="shared" si="35"/>
+        <v>196</v>
+      </c>
+      <c r="B199">
+        <f t="shared" si="36"/>
+        <v>1965</v>
+      </c>
+      <c r="C199">
         <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A152">
-        <f t="shared" si="27"/>
-        <v>149</v>
-      </c>
-      <c r="B152">
+        <v>194045</v>
+      </c>
+      <c r="E199">
         <f t="shared" si="33"/>
-        <v>1495</v>
-      </c>
-      <c r="C152">
-        <f t="shared" ref="C152" si="35">C151+B152</f>
-        <v>112500</v>
-      </c>
-      <c r="E152">
-        <f t="shared" ref="E152" si="36">A152</f>
-        <v>149</v>
-      </c>
-      <c r="F152" t="s">
-        <v>3</v>
-      </c>
-      <c r="G152">
-        <f t="shared" ref="G152" si="37">C152</f>
-        <v>112500</v>
+        <v>196</v>
+      </c>
+      <c r="F199" t="s">
+        <v>3</v>
+      </c>
+      <c r="G199">
+        <f t="shared" si="34"/>
+        <v>194045</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <f t="shared" si="35"/>
+        <v>197</v>
+      </c>
+      <c r="B200">
+        <f t="shared" si="36"/>
+        <v>1975</v>
+      </c>
+      <c r="C200">
+        <f t="shared" si="32"/>
+        <v>196020</v>
+      </c>
+      <c r="E200">
+        <f t="shared" si="33"/>
+        <v>197</v>
+      </c>
+      <c r="F200" t="s">
+        <v>3</v>
+      </c>
+      <c r="G200">
+        <f t="shared" si="34"/>
+        <v>196020</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <f t="shared" si="35"/>
+        <v>198</v>
+      </c>
+      <c r="B201">
+        <f t="shared" si="36"/>
+        <v>1985</v>
+      </c>
+      <c r="C201">
+        <f t="shared" si="32"/>
+        <v>198005</v>
+      </c>
+      <c r="E201">
+        <f t="shared" si="33"/>
+        <v>198</v>
+      </c>
+      <c r="F201" t="s">
+        <v>3</v>
+      </c>
+      <c r="G201">
+        <f t="shared" si="34"/>
+        <v>198005</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <f t="shared" si="35"/>
+        <v>199</v>
+      </c>
+      <c r="B202">
+        <f t="shared" si="36"/>
+        <v>1995</v>
+      </c>
+      <c r="C202">
+        <f t="shared" si="32"/>
+        <v>200000</v>
+      </c>
+      <c r="E202">
+        <f t="shared" si="33"/>
+        <v>199</v>
+      </c>
+      <c r="F202" t="s">
+        <v>3</v>
+      </c>
+      <c r="G202">
+        <f t="shared" si="34"/>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <f t="shared" si="35"/>
+        <v>200</v>
+      </c>
+      <c r="B203">
+        <f t="shared" si="36"/>
+        <v>2005</v>
+      </c>
+      <c r="C203">
+        <f t="shared" si="32"/>
+        <v>202005</v>
+      </c>
+      <c r="E203">
+        <f t="shared" si="33"/>
+        <v>200</v>
+      </c>
+      <c r="F203" t="s">
+        <v>3</v>
+      </c>
+      <c r="G203">
+        <f t="shared" si="34"/>
+        <v>202005</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <f t="shared" si="35"/>
+        <v>201</v>
+      </c>
+      <c r="B204">
+        <f t="shared" si="36"/>
+        <v>2015</v>
+      </c>
+      <c r="C204">
+        <f t="shared" si="32"/>
+        <v>204020</v>
+      </c>
+      <c r="E204">
+        <f t="shared" si="33"/>
+        <v>201</v>
+      </c>
+      <c r="F204" t="s">
+        <v>3</v>
+      </c>
+      <c r="G204">
+        <f t="shared" si="34"/>
+        <v>204020</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <f t="shared" si="35"/>
+        <v>202</v>
+      </c>
+      <c r="B205">
+        <f t="shared" si="36"/>
+        <v>2025</v>
+      </c>
+      <c r="C205">
+        <f t="shared" si="32"/>
+        <v>206045</v>
+      </c>
+      <c r="E205">
+        <f t="shared" si="33"/>
+        <v>202</v>
+      </c>
+      <c r="F205" t="s">
+        <v>3</v>
+      </c>
+      <c r="G205">
+        <f t="shared" si="34"/>
+        <v>206045</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <f t="shared" si="35"/>
+        <v>203</v>
+      </c>
+      <c r="B206">
+        <f t="shared" si="36"/>
+        <v>2035</v>
+      </c>
+      <c r="C206">
+        <f t="shared" si="32"/>
+        <v>208080</v>
+      </c>
+      <c r="E206">
+        <f t="shared" si="33"/>
+        <v>203</v>
+      </c>
+      <c r="F206" t="s">
+        <v>3</v>
+      </c>
+      <c r="G206">
+        <f t="shared" si="34"/>
+        <v>208080</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <f t="shared" si="35"/>
+        <v>204</v>
+      </c>
+      <c r="B207">
+        <f t="shared" si="36"/>
+        <v>2045</v>
+      </c>
+      <c r="C207">
+        <f t="shared" si="32"/>
+        <v>210125</v>
+      </c>
+      <c r="E207">
+        <f t="shared" si="33"/>
+        <v>204</v>
+      </c>
+      <c r="F207" t="s">
+        <v>3</v>
+      </c>
+      <c r="G207">
+        <f t="shared" si="34"/>
+        <v>210125</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <f t="shared" si="35"/>
+        <v>205</v>
+      </c>
+      <c r="B208">
+        <f t="shared" si="36"/>
+        <v>2055</v>
+      </c>
+      <c r="C208">
+        <f t="shared" si="32"/>
+        <v>212180</v>
+      </c>
+      <c r="E208">
+        <f t="shared" si="33"/>
+        <v>205</v>
+      </c>
+      <c r="F208" t="s">
+        <v>3</v>
+      </c>
+      <c r="G208">
+        <f t="shared" si="34"/>
+        <v>212180</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <f t="shared" si="35"/>
+        <v>206</v>
+      </c>
+      <c r="B209">
+        <f t="shared" si="36"/>
+        <v>2065</v>
+      </c>
+      <c r="C209">
+        <f t="shared" si="32"/>
+        <v>214245</v>
+      </c>
+      <c r="E209">
+        <f t="shared" si="33"/>
+        <v>206</v>
+      </c>
+      <c r="F209" t="s">
+        <v>3</v>
+      </c>
+      <c r="G209">
+        <f t="shared" si="34"/>
+        <v>214245</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <f t="shared" si="35"/>
+        <v>207</v>
+      </c>
+      <c r="B210">
+        <f t="shared" si="36"/>
+        <v>2075</v>
+      </c>
+      <c r="C210">
+        <f t="shared" si="32"/>
+        <v>216320</v>
+      </c>
+      <c r="E210">
+        <f t="shared" si="33"/>
+        <v>207</v>
+      </c>
+      <c r="F210" t="s">
+        <v>3</v>
+      </c>
+      <c r="G210">
+        <f t="shared" si="34"/>
+        <v>216320</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <f t="shared" si="35"/>
+        <v>208</v>
+      </c>
+      <c r="B211">
+        <f t="shared" si="36"/>
+        <v>2085</v>
+      </c>
+      <c r="C211">
+        <f t="shared" si="32"/>
+        <v>218405</v>
+      </c>
+      <c r="E211">
+        <f t="shared" si="33"/>
+        <v>208</v>
+      </c>
+      <c r="F211" t="s">
+        <v>3</v>
+      </c>
+      <c r="G211">
+        <f t="shared" si="34"/>
+        <v>218405</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <f t="shared" si="35"/>
+        <v>209</v>
+      </c>
+      <c r="B212">
+        <f t="shared" si="36"/>
+        <v>2095</v>
+      </c>
+      <c r="C212">
+        <f t="shared" si="32"/>
+        <v>220500</v>
+      </c>
+      <c r="E212">
+        <f t="shared" si="33"/>
+        <v>209</v>
+      </c>
+      <c r="F212" t="s">
+        <v>3</v>
+      </c>
+      <c r="G212">
+        <f t="shared" si="34"/>
+        <v>220500</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <f t="shared" si="35"/>
+        <v>210</v>
+      </c>
+      <c r="B213">
+        <f t="shared" si="36"/>
+        <v>2105</v>
+      </c>
+      <c r="C213">
+        <f t="shared" si="32"/>
+        <v>222605</v>
+      </c>
+      <c r="E213">
+        <f t="shared" si="33"/>
+        <v>210</v>
+      </c>
+      <c r="F213" t="s">
+        <v>3</v>
+      </c>
+      <c r="G213">
+        <f t="shared" si="34"/>
+        <v>222605</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <f t="shared" si="35"/>
+        <v>211</v>
+      </c>
+      <c r="B214">
+        <f t="shared" si="36"/>
+        <v>2115</v>
+      </c>
+      <c r="C214">
+        <f t="shared" si="32"/>
+        <v>224720</v>
+      </c>
+      <c r="E214">
+        <f t="shared" si="33"/>
+        <v>211</v>
+      </c>
+      <c r="F214" t="s">
+        <v>3</v>
+      </c>
+      <c r="G214">
+        <f t="shared" si="34"/>
+        <v>224720</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <f t="shared" si="35"/>
+        <v>212</v>
+      </c>
+      <c r="B215">
+        <f t="shared" si="36"/>
+        <v>2125</v>
+      </c>
+      <c r="C215">
+        <f t="shared" si="32"/>
+        <v>226845</v>
+      </c>
+      <c r="E215">
+        <f t="shared" si="33"/>
+        <v>212</v>
+      </c>
+      <c r="F215" t="s">
+        <v>3</v>
+      </c>
+      <c r="G215">
+        <f t="shared" si="34"/>
+        <v>226845</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <f t="shared" si="35"/>
+        <v>213</v>
+      </c>
+      <c r="B216">
+        <f t="shared" si="36"/>
+        <v>2135</v>
+      </c>
+      <c r="C216">
+        <f t="shared" si="32"/>
+        <v>228980</v>
+      </c>
+      <c r="E216">
+        <f t="shared" si="33"/>
+        <v>213</v>
+      </c>
+      <c r="F216" t="s">
+        <v>3</v>
+      </c>
+      <c r="G216">
+        <f t="shared" si="34"/>
+        <v>228980</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <f t="shared" si="35"/>
+        <v>214</v>
+      </c>
+      <c r="B217">
+        <f t="shared" si="36"/>
+        <v>2145</v>
+      </c>
+      <c r="C217">
+        <f t="shared" ref="C217:C280" si="37">C216+B217</f>
+        <v>231125</v>
+      </c>
+      <c r="E217">
+        <f t="shared" ref="E217:E280" si="38">A217</f>
+        <v>214</v>
+      </c>
+      <c r="F217" t="s">
+        <v>3</v>
+      </c>
+      <c r="G217">
+        <f t="shared" ref="G217:G280" si="39">C217</f>
+        <v>231125</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <f t="shared" si="35"/>
+        <v>215</v>
+      </c>
+      <c r="B218">
+        <f t="shared" si="36"/>
+        <v>2155</v>
+      </c>
+      <c r="C218">
+        <f t="shared" si="37"/>
+        <v>233280</v>
+      </c>
+      <c r="E218">
+        <f t="shared" si="38"/>
+        <v>215</v>
+      </c>
+      <c r="F218" t="s">
+        <v>3</v>
+      </c>
+      <c r="G218">
+        <f t="shared" si="39"/>
+        <v>233280</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <f t="shared" si="35"/>
+        <v>216</v>
+      </c>
+      <c r="B219">
+        <f t="shared" si="36"/>
+        <v>2165</v>
+      </c>
+      <c r="C219">
+        <f t="shared" si="37"/>
+        <v>235445</v>
+      </c>
+      <c r="E219">
+        <f t="shared" si="38"/>
+        <v>216</v>
+      </c>
+      <c r="F219" t="s">
+        <v>3</v>
+      </c>
+      <c r="G219">
+        <f t="shared" si="39"/>
+        <v>235445</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <f t="shared" si="35"/>
+        <v>217</v>
+      </c>
+      <c r="B220">
+        <f t="shared" si="36"/>
+        <v>2175</v>
+      </c>
+      <c r="C220">
+        <f t="shared" si="37"/>
+        <v>237620</v>
+      </c>
+      <c r="E220">
+        <f t="shared" si="38"/>
+        <v>217</v>
+      </c>
+      <c r="F220" t="s">
+        <v>3</v>
+      </c>
+      <c r="G220">
+        <f t="shared" si="39"/>
+        <v>237620</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <f t="shared" si="35"/>
+        <v>218</v>
+      </c>
+      <c r="B221">
+        <f t="shared" si="36"/>
+        <v>2185</v>
+      </c>
+      <c r="C221">
+        <f t="shared" si="37"/>
+        <v>239805</v>
+      </c>
+      <c r="E221">
+        <f t="shared" si="38"/>
+        <v>218</v>
+      </c>
+      <c r="F221" t="s">
+        <v>3</v>
+      </c>
+      <c r="G221">
+        <f t="shared" si="39"/>
+        <v>239805</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <f t="shared" si="35"/>
+        <v>219</v>
+      </c>
+      <c r="B222">
+        <f t="shared" si="36"/>
+        <v>2195</v>
+      </c>
+      <c r="C222">
+        <f t="shared" si="37"/>
+        <v>242000</v>
+      </c>
+      <c r="E222">
+        <f t="shared" si="38"/>
+        <v>219</v>
+      </c>
+      <c r="F222" t="s">
+        <v>3</v>
+      </c>
+      <c r="G222">
+        <f t="shared" si="39"/>
+        <v>242000</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <f t="shared" si="35"/>
+        <v>220</v>
+      </c>
+      <c r="B223">
+        <f t="shared" si="36"/>
+        <v>2205</v>
+      </c>
+      <c r="C223">
+        <f t="shared" si="37"/>
+        <v>244205</v>
+      </c>
+      <c r="E223">
+        <f t="shared" si="38"/>
+        <v>220</v>
+      </c>
+      <c r="F223" t="s">
+        <v>3</v>
+      </c>
+      <c r="G223">
+        <f t="shared" si="39"/>
+        <v>244205</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <f t="shared" si="35"/>
+        <v>221</v>
+      </c>
+      <c r="B224">
+        <f t="shared" si="36"/>
+        <v>2215</v>
+      </c>
+      <c r="C224">
+        <f t="shared" si="37"/>
+        <v>246420</v>
+      </c>
+      <c r="E224">
+        <f t="shared" si="38"/>
+        <v>221</v>
+      </c>
+      <c r="F224" t="s">
+        <v>3</v>
+      </c>
+      <c r="G224">
+        <f t="shared" si="39"/>
+        <v>246420</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <f t="shared" si="35"/>
+        <v>222</v>
+      </c>
+      <c r="B225">
+        <f t="shared" si="36"/>
+        <v>2225</v>
+      </c>
+      <c r="C225">
+        <f t="shared" si="37"/>
+        <v>248645</v>
+      </c>
+      <c r="E225">
+        <f t="shared" si="38"/>
+        <v>222</v>
+      </c>
+      <c r="F225" t="s">
+        <v>3</v>
+      </c>
+      <c r="G225">
+        <f t="shared" si="39"/>
+        <v>248645</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <f t="shared" si="35"/>
+        <v>223</v>
+      </c>
+      <c r="B226">
+        <f t="shared" si="36"/>
+        <v>2235</v>
+      </c>
+      <c r="C226">
+        <f t="shared" si="37"/>
+        <v>250880</v>
+      </c>
+      <c r="E226">
+        <f t="shared" si="38"/>
+        <v>223</v>
+      </c>
+      <c r="F226" t="s">
+        <v>3</v>
+      </c>
+      <c r="G226">
+        <f t="shared" si="39"/>
+        <v>250880</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <f t="shared" si="35"/>
+        <v>224</v>
+      </c>
+      <c r="B227">
+        <f t="shared" si="36"/>
+        <v>2245</v>
+      </c>
+      <c r="C227">
+        <f t="shared" si="37"/>
+        <v>253125</v>
+      </c>
+      <c r="E227">
+        <f t="shared" si="38"/>
+        <v>224</v>
+      </c>
+      <c r="F227" t="s">
+        <v>3</v>
+      </c>
+      <c r="G227">
+        <f t="shared" si="39"/>
+        <v>253125</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <f t="shared" si="35"/>
+        <v>225</v>
+      </c>
+      <c r="B228">
+        <f t="shared" si="36"/>
+        <v>2255</v>
+      </c>
+      <c r="C228">
+        <f t="shared" si="37"/>
+        <v>255380</v>
+      </c>
+      <c r="E228">
+        <f t="shared" si="38"/>
+        <v>225</v>
+      </c>
+      <c r="F228" t="s">
+        <v>3</v>
+      </c>
+      <c r="G228">
+        <f t="shared" si="39"/>
+        <v>255380</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <f t="shared" si="35"/>
+        <v>226</v>
+      </c>
+      <c r="B229">
+        <f t="shared" si="36"/>
+        <v>2265</v>
+      </c>
+      <c r="C229">
+        <f t="shared" si="37"/>
+        <v>257645</v>
+      </c>
+      <c r="E229">
+        <f t="shared" si="38"/>
+        <v>226</v>
+      </c>
+      <c r="F229" t="s">
+        <v>3</v>
+      </c>
+      <c r="G229">
+        <f t="shared" si="39"/>
+        <v>257645</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <f t="shared" si="35"/>
+        <v>227</v>
+      </c>
+      <c r="B230">
+        <f t="shared" si="36"/>
+        <v>2275</v>
+      </c>
+      <c r="C230">
+        <f t="shared" si="37"/>
+        <v>259920</v>
+      </c>
+      <c r="E230">
+        <f t="shared" si="38"/>
+        <v>227</v>
+      </c>
+      <c r="F230" t="s">
+        <v>3</v>
+      </c>
+      <c r="G230">
+        <f t="shared" si="39"/>
+        <v>259920</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <f t="shared" si="35"/>
+        <v>228</v>
+      </c>
+      <c r="B231">
+        <f t="shared" si="36"/>
+        <v>2285</v>
+      </c>
+      <c r="C231">
+        <f t="shared" si="37"/>
+        <v>262205</v>
+      </c>
+      <c r="E231">
+        <f t="shared" si="38"/>
+        <v>228</v>
+      </c>
+      <c r="F231" t="s">
+        <v>3</v>
+      </c>
+      <c r="G231">
+        <f t="shared" si="39"/>
+        <v>262205</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <f t="shared" si="35"/>
+        <v>229</v>
+      </c>
+      <c r="B232">
+        <f t="shared" si="36"/>
+        <v>2295</v>
+      </c>
+      <c r="C232">
+        <f t="shared" si="37"/>
+        <v>264500</v>
+      </c>
+      <c r="E232">
+        <f t="shared" si="38"/>
+        <v>229</v>
+      </c>
+      <c r="F232" t="s">
+        <v>3</v>
+      </c>
+      <c r="G232">
+        <f t="shared" si="39"/>
+        <v>264500</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <f t="shared" si="35"/>
+        <v>230</v>
+      </c>
+      <c r="B233">
+        <f t="shared" si="36"/>
+        <v>2305</v>
+      </c>
+      <c r="C233">
+        <f t="shared" si="37"/>
+        <v>266805</v>
+      </c>
+      <c r="E233">
+        <f t="shared" si="38"/>
+        <v>230</v>
+      </c>
+      <c r="F233" t="s">
+        <v>3</v>
+      </c>
+      <c r="G233">
+        <f t="shared" si="39"/>
+        <v>266805</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <f t="shared" si="35"/>
+        <v>231</v>
+      </c>
+      <c r="B234">
+        <f t="shared" si="36"/>
+        <v>2315</v>
+      </c>
+      <c r="C234">
+        <f t="shared" si="37"/>
+        <v>269120</v>
+      </c>
+      <c r="E234">
+        <f t="shared" si="38"/>
+        <v>231</v>
+      </c>
+      <c r="F234" t="s">
+        <v>3</v>
+      </c>
+      <c r="G234">
+        <f t="shared" si="39"/>
+        <v>269120</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <f t="shared" si="35"/>
+        <v>232</v>
+      </c>
+      <c r="B235">
+        <f t="shared" si="36"/>
+        <v>2325</v>
+      </c>
+      <c r="C235">
+        <f t="shared" si="37"/>
+        <v>271445</v>
+      </c>
+      <c r="E235">
+        <f t="shared" si="38"/>
+        <v>232</v>
+      </c>
+      <c r="F235" t="s">
+        <v>3</v>
+      </c>
+      <c r="G235">
+        <f t="shared" si="39"/>
+        <v>271445</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <f t="shared" si="35"/>
+        <v>233</v>
+      </c>
+      <c r="B236">
+        <f t="shared" si="36"/>
+        <v>2335</v>
+      </c>
+      <c r="C236">
+        <f t="shared" si="37"/>
+        <v>273780</v>
+      </c>
+      <c r="E236">
+        <f t="shared" si="38"/>
+        <v>233</v>
+      </c>
+      <c r="F236" t="s">
+        <v>3</v>
+      </c>
+      <c r="G236">
+        <f t="shared" si="39"/>
+        <v>273780</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <f t="shared" si="35"/>
+        <v>234</v>
+      </c>
+      <c r="B237">
+        <f t="shared" si="36"/>
+        <v>2345</v>
+      </c>
+      <c r="C237">
+        <f t="shared" si="37"/>
+        <v>276125</v>
+      </c>
+      <c r="E237">
+        <f t="shared" si="38"/>
+        <v>234</v>
+      </c>
+      <c r="F237" t="s">
+        <v>3</v>
+      </c>
+      <c r="G237">
+        <f t="shared" si="39"/>
+        <v>276125</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <f t="shared" si="35"/>
+        <v>235</v>
+      </c>
+      <c r="B238">
+        <f t="shared" si="36"/>
+        <v>2355</v>
+      </c>
+      <c r="C238">
+        <f t="shared" si="37"/>
+        <v>278480</v>
+      </c>
+      <c r="E238">
+        <f t="shared" si="38"/>
+        <v>235</v>
+      </c>
+      <c r="F238" t="s">
+        <v>3</v>
+      </c>
+      <c r="G238">
+        <f t="shared" si="39"/>
+        <v>278480</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <f t="shared" si="35"/>
+        <v>236</v>
+      </c>
+      <c r="B239">
+        <f t="shared" si="36"/>
+        <v>2365</v>
+      </c>
+      <c r="C239">
+        <f t="shared" si="37"/>
+        <v>280845</v>
+      </c>
+      <c r="E239">
+        <f t="shared" si="38"/>
+        <v>236</v>
+      </c>
+      <c r="F239" t="s">
+        <v>3</v>
+      </c>
+      <c r="G239">
+        <f t="shared" si="39"/>
+        <v>280845</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <f t="shared" si="35"/>
+        <v>237</v>
+      </c>
+      <c r="B240">
+        <f t="shared" si="36"/>
+        <v>2375</v>
+      </c>
+      <c r="C240">
+        <f t="shared" si="37"/>
+        <v>283220</v>
+      </c>
+      <c r="E240">
+        <f t="shared" si="38"/>
+        <v>237</v>
+      </c>
+      <c r="F240" t="s">
+        <v>3</v>
+      </c>
+      <c r="G240">
+        <f t="shared" si="39"/>
+        <v>283220</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <f t="shared" si="35"/>
+        <v>238</v>
+      </c>
+      <c r="B241">
+        <f t="shared" si="36"/>
+        <v>2385</v>
+      </c>
+      <c r="C241">
+        <f t="shared" si="37"/>
+        <v>285605</v>
+      </c>
+      <c r="E241">
+        <f t="shared" si="38"/>
+        <v>238</v>
+      </c>
+      <c r="F241" t="s">
+        <v>3</v>
+      </c>
+      <c r="G241">
+        <f t="shared" si="39"/>
+        <v>285605</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <f t="shared" si="35"/>
+        <v>239</v>
+      </c>
+      <c r="B242">
+        <f t="shared" si="36"/>
+        <v>2395</v>
+      </c>
+      <c r="C242">
+        <f t="shared" si="37"/>
+        <v>288000</v>
+      </c>
+      <c r="E242">
+        <f t="shared" si="38"/>
+        <v>239</v>
+      </c>
+      <c r="F242" t="s">
+        <v>3</v>
+      </c>
+      <c r="G242">
+        <f t="shared" si="39"/>
+        <v>288000</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <f t="shared" si="35"/>
+        <v>240</v>
+      </c>
+      <c r="B243">
+        <f t="shared" si="36"/>
+        <v>2405</v>
+      </c>
+      <c r="C243">
+        <f t="shared" si="37"/>
+        <v>290405</v>
+      </c>
+      <c r="E243">
+        <f t="shared" si="38"/>
+        <v>240</v>
+      </c>
+      <c r="F243" t="s">
+        <v>3</v>
+      </c>
+      <c r="G243">
+        <f t="shared" si="39"/>
+        <v>290405</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <f t="shared" si="35"/>
+        <v>241</v>
+      </c>
+      <c r="B244">
+        <f t="shared" si="36"/>
+        <v>2415</v>
+      </c>
+      <c r="C244">
+        <f t="shared" si="37"/>
+        <v>292820</v>
+      </c>
+      <c r="E244">
+        <f t="shared" si="38"/>
+        <v>241</v>
+      </c>
+      <c r="F244" t="s">
+        <v>3</v>
+      </c>
+      <c r="G244">
+        <f t="shared" si="39"/>
+        <v>292820</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <f t="shared" si="35"/>
+        <v>242</v>
+      </c>
+      <c r="B245">
+        <f t="shared" si="36"/>
+        <v>2425</v>
+      </c>
+      <c r="C245">
+        <f t="shared" si="37"/>
+        <v>295245</v>
+      </c>
+      <c r="E245">
+        <f t="shared" si="38"/>
+        <v>242</v>
+      </c>
+      <c r="F245" t="s">
+        <v>3</v>
+      </c>
+      <c r="G245">
+        <f t="shared" si="39"/>
+        <v>295245</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <f t="shared" si="35"/>
+        <v>243</v>
+      </c>
+      <c r="B246">
+        <f t="shared" si="36"/>
+        <v>2435</v>
+      </c>
+      <c r="C246">
+        <f t="shared" si="37"/>
+        <v>297680</v>
+      </c>
+      <c r="E246">
+        <f t="shared" si="38"/>
+        <v>243</v>
+      </c>
+      <c r="F246" t="s">
+        <v>3</v>
+      </c>
+      <c r="G246">
+        <f t="shared" si="39"/>
+        <v>297680</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <f t="shared" si="35"/>
+        <v>244</v>
+      </c>
+      <c r="B247">
+        <f t="shared" si="36"/>
+        <v>2445</v>
+      </c>
+      <c r="C247">
+        <f t="shared" si="37"/>
+        <v>300125</v>
+      </c>
+      <c r="E247">
+        <f t="shared" si="38"/>
+        <v>244</v>
+      </c>
+      <c r="F247" t="s">
+        <v>3</v>
+      </c>
+      <c r="G247">
+        <f t="shared" si="39"/>
+        <v>300125</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <f t="shared" si="35"/>
+        <v>245</v>
+      </c>
+      <c r="B248">
+        <f t="shared" si="36"/>
+        <v>2455</v>
+      </c>
+      <c r="C248">
+        <f t="shared" si="37"/>
+        <v>302580</v>
+      </c>
+      <c r="E248">
+        <f t="shared" si="38"/>
+        <v>245</v>
+      </c>
+      <c r="F248" t="s">
+        <v>3</v>
+      </c>
+      <c r="G248">
+        <f t="shared" si="39"/>
+        <v>302580</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <f t="shared" si="35"/>
+        <v>246</v>
+      </c>
+      <c r="B249">
+        <f t="shared" si="36"/>
+        <v>2465</v>
+      </c>
+      <c r="C249">
+        <f t="shared" si="37"/>
+        <v>305045</v>
+      </c>
+      <c r="E249">
+        <f t="shared" si="38"/>
+        <v>246</v>
+      </c>
+      <c r="F249" t="s">
+        <v>3</v>
+      </c>
+      <c r="G249">
+        <f t="shared" si="39"/>
+        <v>305045</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <f t="shared" si="35"/>
+        <v>247</v>
+      </c>
+      <c r="B250">
+        <f t="shared" si="36"/>
+        <v>2475</v>
+      </c>
+      <c r="C250">
+        <f t="shared" si="37"/>
+        <v>307520</v>
+      </c>
+      <c r="E250">
+        <f t="shared" si="38"/>
+        <v>247</v>
+      </c>
+      <c r="F250" t="s">
+        <v>3</v>
+      </c>
+      <c r="G250">
+        <f t="shared" si="39"/>
+        <v>307520</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <f t="shared" si="35"/>
+        <v>248</v>
+      </c>
+      <c r="B251">
+        <f t="shared" si="36"/>
+        <v>2485</v>
+      </c>
+      <c r="C251">
+        <f t="shared" si="37"/>
+        <v>310005</v>
+      </c>
+      <c r="E251">
+        <f t="shared" si="38"/>
+        <v>248</v>
+      </c>
+      <c r="F251" t="s">
+        <v>3</v>
+      </c>
+      <c r="G251">
+        <f t="shared" si="39"/>
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <f t="shared" si="35"/>
+        <v>249</v>
+      </c>
+      <c r="B252">
+        <f t="shared" si="36"/>
+        <v>2495</v>
+      </c>
+      <c r="C252">
+        <f t="shared" si="37"/>
+        <v>312500</v>
+      </c>
+      <c r="E252">
+        <f t="shared" si="38"/>
+        <v>249</v>
+      </c>
+      <c r="F252" t="s">
+        <v>3</v>
+      </c>
+      <c r="G252">
+        <f t="shared" si="39"/>
+        <v>312500</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <f t="shared" si="35"/>
+        <v>250</v>
+      </c>
+      <c r="B253">
+        <f t="shared" si="36"/>
+        <v>2505</v>
+      </c>
+      <c r="C253">
+        <f t="shared" si="37"/>
+        <v>315005</v>
+      </c>
+      <c r="E253">
+        <f t="shared" si="38"/>
+        <v>250</v>
+      </c>
+      <c r="F253" t="s">
+        <v>3</v>
+      </c>
+      <c r="G253">
+        <f t="shared" si="39"/>
+        <v>315005</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <f t="shared" si="35"/>
+        <v>251</v>
+      </c>
+      <c r="B254">
+        <f t="shared" si="36"/>
+        <v>2515</v>
+      </c>
+      <c r="C254">
+        <f t="shared" si="37"/>
+        <v>317520</v>
+      </c>
+      <c r="E254">
+        <f t="shared" si="38"/>
+        <v>251</v>
+      </c>
+      <c r="F254" t="s">
+        <v>3</v>
+      </c>
+      <c r="G254">
+        <f t="shared" si="39"/>
+        <v>317520</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <f t="shared" si="35"/>
+        <v>252</v>
+      </c>
+      <c r="B255">
+        <f t="shared" si="36"/>
+        <v>2525</v>
+      </c>
+      <c r="C255">
+        <f t="shared" si="37"/>
+        <v>320045</v>
+      </c>
+      <c r="E255">
+        <f t="shared" si="38"/>
+        <v>252</v>
+      </c>
+      <c r="F255" t="s">
+        <v>3</v>
+      </c>
+      <c r="G255">
+        <f t="shared" si="39"/>
+        <v>320045</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <f t="shared" si="35"/>
+        <v>253</v>
+      </c>
+      <c r="B256">
+        <f t="shared" si="36"/>
+        <v>2535</v>
+      </c>
+      <c r="C256">
+        <f t="shared" si="37"/>
+        <v>322580</v>
+      </c>
+      <c r="E256">
+        <f t="shared" si="38"/>
+        <v>253</v>
+      </c>
+      <c r="F256" t="s">
+        <v>3</v>
+      </c>
+      <c r="G256">
+        <f t="shared" si="39"/>
+        <v>322580</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <f t="shared" si="35"/>
+        <v>254</v>
+      </c>
+      <c r="B257">
+        <f t="shared" si="36"/>
+        <v>2545</v>
+      </c>
+      <c r="C257">
+        <f t="shared" si="37"/>
+        <v>325125</v>
+      </c>
+      <c r="E257">
+        <f t="shared" si="38"/>
+        <v>254</v>
+      </c>
+      <c r="F257" t="s">
+        <v>3</v>
+      </c>
+      <c r="G257">
+        <f t="shared" si="39"/>
+        <v>325125</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <f t="shared" si="35"/>
+        <v>255</v>
+      </c>
+      <c r="B258">
+        <f t="shared" si="36"/>
+        <v>2555</v>
+      </c>
+      <c r="C258">
+        <f t="shared" si="37"/>
+        <v>327680</v>
+      </c>
+      <c r="E258">
+        <f t="shared" si="38"/>
+        <v>255</v>
+      </c>
+      <c r="F258" t="s">
+        <v>3</v>
+      </c>
+      <c r="G258">
+        <f t="shared" si="39"/>
+        <v>327680</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <f t="shared" si="35"/>
+        <v>256</v>
+      </c>
+      <c r="B259">
+        <f t="shared" si="36"/>
+        <v>2565</v>
+      </c>
+      <c r="C259">
+        <f t="shared" si="37"/>
+        <v>330245</v>
+      </c>
+      <c r="E259">
+        <f t="shared" si="38"/>
+        <v>256</v>
+      </c>
+      <c r="F259" t="s">
+        <v>3</v>
+      </c>
+      <c r="G259">
+        <f t="shared" si="39"/>
+        <v>330245</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <f t="shared" si="35"/>
+        <v>257</v>
+      </c>
+      <c r="B260">
+        <f t="shared" si="36"/>
+        <v>2575</v>
+      </c>
+      <c r="C260">
+        <f t="shared" si="37"/>
+        <v>332820</v>
+      </c>
+      <c r="E260">
+        <f t="shared" si="38"/>
+        <v>257</v>
+      </c>
+      <c r="F260" t="s">
+        <v>3</v>
+      </c>
+      <c r="G260">
+        <f t="shared" si="39"/>
+        <v>332820</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <f t="shared" ref="A261:A310" si="40">A260+1</f>
+        <v>258</v>
+      </c>
+      <c r="B261">
+        <f t="shared" si="36"/>
+        <v>2585</v>
+      </c>
+      <c r="C261">
+        <f t="shared" si="37"/>
+        <v>335405</v>
+      </c>
+      <c r="E261">
+        <f t="shared" si="38"/>
+        <v>258</v>
+      </c>
+      <c r="F261" t="s">
+        <v>3</v>
+      </c>
+      <c r="G261">
+        <f t="shared" si="39"/>
+        <v>335405</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <f t="shared" si="40"/>
+        <v>259</v>
+      </c>
+      <c r="B262">
+        <f t="shared" ref="B262:B310" si="41">B261-B260+B261</f>
+        <v>2595</v>
+      </c>
+      <c r="C262">
+        <f t="shared" si="37"/>
+        <v>338000</v>
+      </c>
+      <c r="E262">
+        <f t="shared" si="38"/>
+        <v>259</v>
+      </c>
+      <c r="F262" t="s">
+        <v>3</v>
+      </c>
+      <c r="G262">
+        <f t="shared" si="39"/>
+        <v>338000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>